<commit_message>
vault backup: 2025-03-18 12:45:03
</commit_message>
<xml_diff>
--- a/doc/授课时间表_0315.xlsx
+++ b/doc/授课时间表_0315.xlsx
@@ -114,6 +114,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>1. 模型下载:演示模型下载的方法,实际上提前发给他们压缩包,然后当场他们传云服务器,但是这也很花时间</t>
     </r>
     <r>
@@ -163,6 +169,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>1. 解释大模型的基本原理及其幻觉问题。</t>
     </r>
     <r>
@@ -218,6 +230,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>1. 解释RAG的定义、作用、适用场景及其经典结构。</t>
     </r>
     <r>
@@ -248,6 +266,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>医疗器械法规审核-仓库管理-是否违反防虫防鼠条例</t>
     </r>
     <r>
@@ -281,6 +305,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>医疗器械法规审核-仓库管理-是否违反防虫防鼠条例</t>
     </r>
     <r>
@@ -308,6 +338,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>1. 使用Deepseek模型生成合成数据，扩展训练数据集。</t>
     </r>
     <r>
@@ -1758,12 +1794,13 @@
   <sheetPr/>
   <dimension ref="B1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
   <cols>
+    <col min="3" max="3" width="15.3909090909091" customWidth="1"/>
     <col min="5" max="5" width="23.1181818181818" customWidth="1"/>
     <col min="6" max="6" width="57.9181818181818" customWidth="1"/>
     <col min="10" max="10" width="85.4545454545455" customWidth="1"/>
@@ -1895,7 +1932,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" ht="104" customHeight="1" spans="2:10">
+    <row r="7" ht="86" customHeight="1" spans="2:10">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="8"/>
@@ -1916,7 +1953,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" ht="79" customHeight="1" spans="2:10">
+    <row r="8" ht="58" customHeight="1" spans="2:10">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="8" t="s">
@@ -1964,7 +2001,7 @@
       </c>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" ht="78" customHeight="1" spans="2:10">
+    <row r="10" ht="40" customHeight="1" spans="2:10">
       <c r="B10" s="4"/>
       <c r="C10" s="11"/>
       <c r="D10" s="8"/>
@@ -1985,7 +2022,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" ht="56.75" spans="2:10">
+    <row r="11" ht="65" customHeight="1" spans="2:10">
       <c r="B11" s="4"/>
       <c r="C11" s="11"/>
       <c r="D11" s="8" t="s">
@@ -2008,7 +2045,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" ht="97" customHeight="1" spans="2:10">
+    <row r="12" ht="51" customHeight="1" spans="2:10">
       <c r="B12" s="4"/>
       <c r="C12" s="11"/>
       <c r="D12" s="8"/>
@@ -2052,7 +2089,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" ht="84.75" spans="2:10">
+    <row r="14" ht="14.75" spans="2:10">
       <c r="B14" s="4"/>
       <c r="C14" s="11"/>
       <c r="D14" s="8"/>
@@ -2094,7 +2131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" ht="95" customHeight="1" spans="2:10">
+    <row r="16" ht="55" customHeight="1" spans="2:10">
       <c r="B16" s="4"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12" t="s">

</xml_diff>

<commit_message>
vault backup: 2025-03-18 14:08:28
</commit_message>
<xml_diff>
--- a/doc/授课时间表_0315.xlsx
+++ b/doc/授课时间表_0315.xlsx
@@ -113,53 +113,9 @@
     <t>探索常用社区资源如Github/Huggingface/Modelscope，如何进行模型下载，并通过VLLM/Ollama/SGLang/Transformer启动模型，进行模型试用。</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1. 模型下载:演示模型下载的方法,实际上提前发给他们压缩包,然后当场他们传云服务器,但是这也很花时间</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>2. 模型的部署最基础是transformer启动, 但ds系列不兼容transformer启动,但是后续自己开发的话transformer启动得讲</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>3. vllm启动, ollama启动, SGLang启动, 如果现场配置的话两三小时多不一定搞得定, 但是提前配置docker能上传云服务器就快很多</t>
-    </r>
+    <t>1. 模型下载:演示模型下载的方法,实际上提前发给他们压缩包,然后当场他们传云服务器,但是这也很花时间
+2. 模型的部署最基础是transformer启动, 但ds系列不兼容transformer启动,但是后续自己开发的话transformer启动得讲
+3. vllm启动, ollama启动, SGLang启动, 如果现场配置的话两三小时多不一定搞得定, 但是提前配置docker能上传云服务器就快很多</t>
   </si>
   <si>
     <t>基础使用</t>
@@ -575,7 +531,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,6 +541,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD2F4F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,7 +1047,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1103,16 +1071,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1121,89 +1089,89 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1233,6 +1201,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1794,8 +1768,8 @@
   <sheetPr/>
   <dimension ref="B1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -1832,7 +1806,7 @@
       <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="16" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1858,10 +1832,10 @@
       <c r="H3" s="7">
         <v>20</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="17">
         <v>175</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1883,8 +1857,8 @@
       <c r="H4" s="9">
         <v>20</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="17" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="19" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1895,7 +1869,7 @@
       <c r="E5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -1904,8 +1878,8 @@
       <c r="H5" s="9">
         <v>20</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="17" t="s">
+      <c r="I5" s="17"/>
+      <c r="J5" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1927,8 +1901,8 @@
       <c r="H6" s="9">
         <v>30</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="17"/>
+      <c r="J6" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1939,7 +1913,7 @@
       <c r="E7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -1948,8 +1922,8 @@
       <c r="H7" s="9">
         <v>35</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="18" t="s">
+      <c r="I7" s="17"/>
+      <c r="J7" s="20" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1962,7 +1936,7 @@
       <c r="E8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="12" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -1971,14 +1945,14 @@
       <c r="H8" s="9">
         <v>50</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="18" t="s">
+      <c r="I8" s="17"/>
+      <c r="J8" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" ht="28.75" spans="2:10">
       <c r="B9" s="4"/>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -1987,7 +1961,7 @@
       <c r="E9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="12" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -1996,19 +1970,19 @@
       <c r="H9" s="9">
         <v>75</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="21">
         <v>255</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" ht="40" customHeight="1" spans="2:10">
       <c r="B10" s="4"/>
-      <c r="C10" s="11"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="12" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -2017,21 +1991,21 @@
       <c r="H10" s="9">
         <v>20</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="18" t="s">
+      <c r="I10" s="21"/>
+      <c r="J10" s="20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" ht="65" customHeight="1" spans="2:10">
       <c r="B11" s="4"/>
-      <c r="C11" s="11"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -2040,19 +2014,19 @@
       <c r="H11" s="9">
         <v>40</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="18" t="s">
+      <c r="I11" s="21"/>
+      <c r="J11" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" ht="51" customHeight="1" spans="2:10">
       <c r="B12" s="4"/>
-      <c r="C12" s="11"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="8"/>
       <c r="E12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="12" t="s">
         <v>45</v>
       </c>
       <c r="G12" s="9" t="s">
@@ -2061,21 +2035,21 @@
       <c r="H12" s="9">
         <v>20</v>
       </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="17" t="s">
+      <c r="I12" s="21"/>
+      <c r="J12" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" ht="14.75" spans="2:10">
       <c r="B13" s="4"/>
-      <c r="C13" s="11"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="9" t="s">
@@ -2084,19 +2058,19 @@
       <c r="H13" s="9">
         <v>50</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="17" t="s">
+      <c r="I13" s="21"/>
+      <c r="J13" s="19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" ht="14.75" spans="2:10">
       <c r="B14" s="4"/>
-      <c r="C14" s="11"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="12" t="s">
         <v>52</v>
       </c>
       <c r="G14" s="9" t="s">
@@ -2105,19 +2079,19 @@
       <c r="H14" s="9">
         <v>25</v>
       </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="17" t="s">
+      <c r="I14" s="21"/>
+      <c r="J14" s="19" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" ht="14.75" spans="2:10">
       <c r="B15" s="4"/>
-      <c r="C15" s="11"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="12" t="s">
         <v>55</v>
       </c>
       <c r="G15" s="9" t="s">
@@ -2126,31 +2100,31 @@
       <c r="H15" s="9">
         <v>10</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="17" t="s">
+      <c r="I15" s="21"/>
+      <c r="J15" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" ht="55" customHeight="1" spans="2:10">
       <c r="B16" s="4"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="15">
         <v>15</v>
       </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="22" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>